<commit_message>
Spinners and fixed registration bugs
</commit_message>
<xml_diff>
--- a/Company.xlsx
+++ b/Company.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
-    <sheet name="Query" sheetId="2" r:id="rId2"/>
+    <sheet name="Masters" sheetId="3" r:id="rId2"/>
+    <sheet name="Query" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="279">
   <si>
     <t>Старое название</t>
   </si>
@@ -778,12 +779,99 @@
   <si>
     <t>Govt</t>
   </si>
+  <si>
+    <t>torgrim</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>njkcnbxtkkj</t>
+  </si>
+  <si>
+    <t>Торгрим</t>
+  </si>
+  <si>
+    <t>Энди</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Николя</t>
+  </si>
+  <si>
+    <t>Молидеус</t>
+  </si>
+  <si>
+    <t>bpnjcnthf</t>
+  </si>
+  <si>
+    <t>Толчок</t>
+  </si>
+  <si>
+    <t>Логин</t>
+  </si>
+  <si>
+    <t>Пароль</t>
+  </si>
+  <si>
+    <t>Роль</t>
+  </si>
+  <si>
+    <t>Деньги</t>
+  </si>
+  <si>
+    <t>Заведен</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>A.L.I.C.E</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Вася Кибержокей</t>
+  </si>
+  <si>
+    <t>test_hacker</t>
+  </si>
+  <si>
+    <t>fggdhdr654</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Darknet</t>
+  </si>
+  <si>
+    <t>darknet</t>
+  </si>
+  <si>
+    <t>test_victim</t>
+  </si>
+  <si>
+    <t>Бедная Кисонька</t>
+  </si>
+  <si>
+    <t>alice</t>
+  </si>
+  <si>
+    <t>mechanus7534</t>
+  </si>
+  <si>
+    <t>Администрация</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -848,6 +936,12 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF880000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -915,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -973,6 +1067,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1289,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4418,7 +4518,10 @@
       <c r="D81" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="E81" s="22"/>
+      <c r="E81" s="23" t="str">
+        <f>Query!$A$1 &amp; D81 &amp; Query!$A$2 &amp; B81 &amp; Query!$A$3</f>
+        <v>insert into dbo.Accounts ([Login], PasswordHash, TokenSalt, [Role], Cash, [Status], Insurance, InsuranceLevel, Fullname, [Index], InsurancePoints, InsuranceHidden) values ('Govt', CONVERT(varchar(36), NEWID()), NEWID(), 32, 10000, 1, 0, 0, 'SunLight/government', 0, 0, 0);</v>
+      </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -29393,10 +29496,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="30" customFormat="1">
+      <c r="A1" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2">
+        <v>1000000</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6">
+        <v>60000</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13">
+      <c r="A8" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
AliceInsurance + Registration bug
</commit_message>
<xml_diff>
--- a/Company.xlsx
+++ b/Company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="285">
   <si>
     <t>Старое название</t>
   </si>
@@ -866,6 +866,31 @@
   <si>
     <t>Администрация</t>
   </si>
+  <si>
+    <t>Хелпдеск</t>
+  </si>
+  <si>
+    <t>Helpdesk</t>
+  </si>
+  <si>
+    <t>helpdesk</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>hdhdhd333</t>
+  </si>
+  <si>
+    <t>select [Login], [Role], total10, total50, total200 from dbo.Accounts 
+left outer join (select count(*) as total10, Employer from dbo.Payments where Amount = 10 group by employer) as t10
+on [Login] = t10.Employer
+left outer join (select count(*) as total50, Employer from dbo.Payments where Amount = 50 group by employer) as t50
+on [Login] = t50.Employer
+left outer join (select count(*) as total200, Employer from dbo.Payments where Amount = 200 group by employer) as t200
+on [Login] = t200.Employer
+ where [Role] &gt; 4 order by [Login];</t>
+  </si>
 </sst>
 </file>
 
@@ -1009,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1071,6 +1096,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1389,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
@@ -1447,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="str">
-        <f>C2</f>
+        <f t="shared" ref="D2:D40" si="0">C2</f>
         <v>amcoffee</v>
       </c>
       <c r="E2" s="23" t="str">
@@ -1486,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f>C3</f>
+        <f t="shared" si="0"/>
         <v>clubhell</v>
       </c>
       <c r="E3" s="23" t="str">
@@ -1525,7 +1553,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>tangobar</v>
       </c>
       <c r="E4" s="23" t="str">
@@ -1564,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>cbs13</v>
       </c>
       <c r="E5" s="23" t="str">
@@ -1603,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>orthchurch</v>
       </c>
       <c r="E6" s="23" t="str">
@@ -1642,7 +1670,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>searchag</v>
       </c>
       <c r="E7" s="23" t="str">
@@ -1681,7 +1709,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>solag</v>
       </c>
       <c r="E8" s="23" t="str">
@@ -1720,7 +1748,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>lightag</v>
       </c>
       <c r="E9" s="23" t="str">
@@ -1759,7 +1787,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>fimsag</v>
       </c>
       <c r="E10" s="23" t="str">
@@ -1798,7 +1826,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>johnsonadm</v>
       </c>
       <c r="E11" s="23" t="str">
@@ -1837,7 +1865,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>serenityadm</v>
       </c>
       <c r="E12" s="23" t="str">
@@ -1876,7 +1904,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="str">
-        <f>C13</f>
+        <f t="shared" si="0"/>
         <v>deatharena</v>
       </c>
       <c r="E13" s="23" t="str">
@@ -1915,7 +1943,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f>C14</f>
+        <f t="shared" si="0"/>
         <v>arenacol</v>
       </c>
       <c r="E14" s="23" t="str">
@@ -1954,7 +1982,7 @@
         <v>42</v>
       </c>
       <c r="D15" s="2" t="str">
-        <f>C15</f>
+        <f t="shared" si="0"/>
         <v>twilightpub</v>
       </c>
       <c r="E15" s="23" t="str">
@@ -1993,7 +2021,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="2" t="str">
-        <f>C16</f>
+        <f t="shared" si="0"/>
         <v>charitycab</v>
       </c>
       <c r="E16" s="23" t="str">
@@ -2032,7 +2060,7 @@
         <v>48</v>
       </c>
       <c r="D17" s="2" t="str">
-        <f>C17</f>
+        <f t="shared" si="0"/>
         <v>fundrebirth</v>
       </c>
       <c r="E17" s="23" t="str">
@@ -2071,7 +2099,7 @@
         <v>51</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f>C18</f>
+        <f t="shared" si="0"/>
         <v>crimcloud</v>
       </c>
       <c r="E18" s="23" t="str">
@@ -2110,7 +2138,7 @@
         <v>54</v>
       </c>
       <c r="D19" s="2" t="str">
-        <f>C19</f>
+        <f t="shared" si="0"/>
         <v>vapeclub</v>
       </c>
       <c r="E19" s="23" t="str">
@@ -2149,7 +2177,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="2" t="str">
-        <f>C20</f>
+        <f t="shared" si="0"/>
         <v>garagecoop</v>
       </c>
       <c r="E20" s="23" t="str">
@@ -2188,7 +2216,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f>C21</f>
+        <f t="shared" si="0"/>
         <v>sfpolice</v>
       </c>
       <c r="E21" s="23" t="str">
@@ -2227,7 +2255,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="2" t="str">
-        <f>C22</f>
+        <f t="shared" si="0"/>
         <v>pivalentine</v>
       </c>
       <c r="E22" s="23" t="str">
@@ -2266,7 +2294,7 @@
         <v>65</v>
       </c>
       <c r="D23" s="2" t="str">
-        <f>C23</f>
+        <f t="shared" si="0"/>
         <v>pitokanava</v>
       </c>
       <c r="E23" s="23" t="str">
@@ -2305,7 +2333,7 @@
         <v>67</v>
       </c>
       <c r="D24" s="2" t="str">
-        <f>C24</f>
+        <f t="shared" si="0"/>
         <v>engincom</v>
       </c>
       <c r="E24" s="23" t="str">
@@ -2344,7 +2372,7 @@
         <v>70</v>
       </c>
       <c r="D25" s="2" t="str">
-        <f>C25</f>
+        <f t="shared" si="0"/>
         <v>masonpub</v>
       </c>
       <c r="E25" s="23" t="str">
@@ -2383,7 +2411,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="2" t="str">
-        <f>C26</f>
+        <f t="shared" si="0"/>
         <v>capshost</v>
       </c>
       <c r="E26" s="23" t="str">
@@ -2422,7 +2450,7 @@
         <v>74</v>
       </c>
       <c r="D27" s="2" t="str">
-        <f>C27</f>
+        <f t="shared" si="0"/>
         <v>lightcafe</v>
       </c>
       <c r="E27" s="23" t="str">
@@ -2461,7 +2489,7 @@
         <v>76</v>
       </c>
       <c r="D28" s="2" t="str">
-        <f>C28</f>
+        <f t="shared" si="0"/>
         <v>elysclub</v>
       </c>
       <c r="E28" s="23" t="str">
@@ -2500,7 +2528,7 @@
         <v>78</v>
       </c>
       <c r="D29" s="2" t="str">
-        <f>C29</f>
+        <f t="shared" si="0"/>
         <v>columb</v>
       </c>
       <c r="E29" s="23" t="str">
@@ -2539,7 +2567,7 @@
         <v>81</v>
       </c>
       <c r="D30" s="2" t="str">
-        <f>C30</f>
+        <f t="shared" si="0"/>
         <v>rescuecom</v>
       </c>
       <c r="E30" s="23" t="str">
@@ -2578,7 +2606,7 @@
         <v>84</v>
       </c>
       <c r="D31" s="2" t="str">
-        <f>C31</f>
+        <f t="shared" si="0"/>
         <v>securcom</v>
       </c>
       <c r="E31" s="23" t="str">
@@ -2617,7 +2645,7 @@
         <v>87</v>
       </c>
       <c r="D32" s="2" t="str">
-        <f>C32</f>
+        <f t="shared" si="0"/>
         <v>solidcom</v>
       </c>
       <c r="E32" s="23" t="str">
@@ -2656,7 +2684,7 @@
         <v>89</v>
       </c>
       <c r="D33" s="2" t="str">
-        <f>C33</f>
+        <f t="shared" si="0"/>
         <v>arasinc</v>
       </c>
       <c r="E33" s="23" t="str">
@@ -2695,7 +2723,7 @@
         <v>91</v>
       </c>
       <c r="D34" s="2" t="str">
-        <f>C34</f>
+        <f t="shared" si="0"/>
         <v>dexcomp</v>
       </c>
       <c r="E34" s="23" t="str">
@@ -2734,7 +2762,7 @@
         <v>93</v>
       </c>
       <c r="D35" s="2" t="str">
-        <f>C35</f>
+        <f t="shared" si="0"/>
         <v>joycorp</v>
       </c>
       <c r="E35" s="23" t="str">
@@ -2773,7 +2801,7 @@
         <v>96</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f>C36</f>
+        <f t="shared" si="0"/>
         <v>kintsugicorp</v>
       </c>
       <c r="E36" s="23" t="str">
@@ -2812,7 +2840,7 @@
         <v>98</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f>C37</f>
+        <f t="shared" si="0"/>
         <v>opensource</v>
       </c>
       <c r="E37" s="23" t="str">
@@ -2851,7 +2879,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>C38</f>
+        <f t="shared" si="0"/>
         <v>sunlight</v>
       </c>
       <c r="E38" s="23" t="str">
@@ -2890,7 +2918,7 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="str">
-        <f>C39</f>
+        <f t="shared" si="0"/>
         <v>exitclub</v>
       </c>
       <c r="E39" s="23" t="str">
@@ -2929,7 +2957,7 @@
         <v>106</v>
       </c>
       <c r="D40" s="2" t="str">
-        <f>C40</f>
+        <f t="shared" si="0"/>
         <v>serenitycourt</v>
       </c>
       <c r="E40" s="23" t="str">
@@ -3073,7 +3101,7 @@
         <v>117</v>
       </c>
       <c r="D44" s="2" t="str">
-        <f>C44</f>
+        <f t="shared" ref="D44:D80" si="1">C44</f>
         <v>lifescanlab</v>
       </c>
       <c r="E44" s="23" t="str">
@@ -3112,7 +3140,7 @@
         <v>120</v>
       </c>
       <c r="D45" s="2" t="str">
-        <f>C45</f>
+        <f t="shared" si="1"/>
         <v>karhallab</v>
       </c>
       <c r="E45" s="23" t="str">
@@ -3151,7 +3179,7 @@
         <v>123</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f>C46</f>
+        <f t="shared" si="1"/>
         <v>cosmolab</v>
       </c>
       <c r="E46" s="23" t="str">
@@ -3190,7 +3218,7 @@
         <v>126</v>
       </c>
       <c r="D47" s="2" t="str">
-        <f>C47</f>
+        <f t="shared" si="1"/>
         <v>infinity</v>
       </c>
       <c r="E47" s="23" t="str">
@@ -3229,7 +3257,7 @@
         <v>128</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f>C48</f>
+        <f t="shared" si="1"/>
         <v>spanglish</v>
       </c>
       <c r="E48" s="23" t="str">
@@ -3268,7 +3296,7 @@
         <v>131</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f>C49</f>
+        <f t="shared" si="1"/>
         <v>stfranhosp</v>
       </c>
       <c r="E49" s="23" t="str">
@@ -3307,7 +3335,7 @@
         <v>133</v>
       </c>
       <c r="D50" s="2" t="str">
-        <f>C50</f>
+        <f t="shared" si="1"/>
         <v>jailmotel</v>
       </c>
       <c r="E50" s="23" t="str">
@@ -3346,7 +3374,7 @@
         <v>136</v>
       </c>
       <c r="D51" s="2" t="str">
-        <f>C51</f>
+        <f t="shared" si="1"/>
         <v>activdtown</v>
       </c>
       <c r="E51" s="23" t="str">
@@ -3385,7 +3413,7 @@
         <v>139</v>
       </c>
       <c r="D52" s="2" t="str">
-        <f>C52</f>
+        <f t="shared" si="1"/>
         <v>dinastyclub</v>
       </c>
       <c r="E52" s="23" t="str">
@@ -3424,7 +3452,7 @@
         <v>142</v>
       </c>
       <c r="D53" s="2" t="str">
-        <f>C53</f>
+        <f t="shared" si="1"/>
         <v>pornstudio</v>
       </c>
       <c r="E53" s="23" t="str">
@@ -3463,7 +3491,7 @@
         <v>145</v>
       </c>
       <c r="D54" s="2" t="str">
-        <f>C54</f>
+        <f t="shared" si="1"/>
         <v>ghostcorp</v>
       </c>
       <c r="E54" s="23" t="str">
@@ -3502,7 +3530,7 @@
         <v>148</v>
       </c>
       <c r="D55" s="2" t="str">
-        <f>C55</f>
+        <f t="shared" si="1"/>
         <v>isracorp</v>
       </c>
       <c r="E55" s="23" t="str">
@@ -3541,7 +3569,7 @@
         <v>151</v>
       </c>
       <c r="D56" s="2" t="str">
-        <f>C56</f>
+        <f t="shared" si="1"/>
         <v>sistersmith</v>
       </c>
       <c r="E56" s="23" t="str">
@@ -3580,7 +3608,7 @@
         <v>154</v>
       </c>
       <c r="D57" s="2" t="str">
-        <f>C57</f>
+        <f t="shared" si="1"/>
         <v>thirdpub</v>
       </c>
       <c r="E57" s="23" t="str">
@@ -3619,7 +3647,7 @@
         <v>156</v>
       </c>
       <c r="D58" s="2" t="str">
-        <f>C58</f>
+        <f t="shared" si="1"/>
         <v>salon42</v>
       </c>
       <c r="E58" s="23" t="str">
@@ -3658,7 +3686,7 @@
         <v>158</v>
       </c>
       <c r="D59" s="2" t="str">
-        <f>C59</f>
+        <f t="shared" si="1"/>
         <v>brainstorm</v>
       </c>
       <c r="E59" s="23" t="str">
@@ -3697,7 +3725,7 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="str">
-        <f>C60</f>
+        <f t="shared" si="1"/>
         <v>cryskin</v>
       </c>
       <c r="E60" s="23" t="str">
@@ -3736,7 +3764,7 @@
         <v>162</v>
       </c>
       <c r="D61" s="2" t="str">
-        <f>C61</f>
+        <f t="shared" si="1"/>
         <v>dextazy</v>
       </c>
       <c r="E61" s="23" t="str">
@@ -3775,7 +3803,7 @@
         <v>164</v>
       </c>
       <c r="D62" s="2" t="str">
-        <f>C62</f>
+        <f t="shared" si="1"/>
         <v>servcenter</v>
       </c>
       <c r="E62" s="23" t="str">
@@ -3814,7 +3842,7 @@
         <v>166</v>
       </c>
       <c r="D63" s="2" t="str">
-        <f>C63</f>
+        <f t="shared" si="1"/>
         <v>spacity</v>
       </c>
       <c r="E63" s="23" t="str">
@@ -3853,7 +3881,7 @@
         <v>169</v>
       </c>
       <c r="D64" s="2" t="str">
-        <f>C64</f>
+        <f t="shared" si="1"/>
         <v>tatneedle</v>
       </c>
       <c r="E64" s="23" t="str">
@@ -3892,7 +3920,7 @@
         <v>172</v>
       </c>
       <c r="D65" s="2" t="str">
-        <f>C65</f>
+        <f t="shared" si="1"/>
         <v>tatice</v>
       </c>
       <c r="E65" s="23" t="str">
@@ -3931,7 +3959,7 @@
         <v>175</v>
       </c>
       <c r="D66" s="2" t="str">
-        <f>C66</f>
+        <f t="shared" si="1"/>
         <v>janslab</v>
       </c>
       <c r="E66" s="23" t="str">
@@ -3970,7 +3998,7 @@
         <v>178</v>
       </c>
       <c r="D67" s="2" t="str">
-        <f>C67</f>
+        <f t="shared" si="1"/>
         <v>fedcybex</v>
       </c>
       <c r="E67" s="23" t="str">
@@ -4009,7 +4037,7 @@
         <v>180</v>
       </c>
       <c r="D68" s="2" t="str">
-        <f>C68</f>
+        <f t="shared" si="1"/>
         <v>senstore</v>
       </c>
       <c r="E68" s="23" t="str">
@@ -4048,7 +4076,7 @@
         <v>183</v>
       </c>
       <c r="D69" s="2" t="str">
-        <f>C69</f>
+        <f t="shared" si="1"/>
         <v>jjchurch</v>
       </c>
       <c r="E69" s="23" t="str">
@@ -4087,7 +4115,7 @@
         <v>186</v>
       </c>
       <c r="D70" s="2" t="str">
-        <f>C70</f>
+        <f t="shared" si="1"/>
         <v>stregchurch</v>
       </c>
       <c r="E70" s="23" t="str">
@@ -4126,7 +4154,7 @@
         <v>189</v>
       </c>
       <c r="D71" s="2" t="str">
-        <f>C71</f>
+        <f t="shared" si="1"/>
         <v>robocirc</v>
       </c>
       <c r="E71" s="23" t="str">
@@ -4165,7 +4193,7 @@
         <v>192</v>
       </c>
       <c r="D72" s="2" t="str">
-        <f>C72</f>
+        <f t="shared" si="1"/>
         <v>teaseren</v>
       </c>
       <c r="E72" s="23" t="str">
@@ -4204,7 +4232,7 @@
         <v>195</v>
       </c>
       <c r="D73" s="2" t="str">
-        <f>C73</f>
+        <f t="shared" si="1"/>
         <v>excollege</v>
       </c>
       <c r="E73" s="23" t="str">
@@ -4243,7 +4271,7 @@
         <v>197</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f>C74</f>
+        <f t="shared" si="1"/>
         <v>legalcom</v>
       </c>
       <c r="E74" s="23" t="str">
@@ -4282,7 +4310,7 @@
         <v>200</v>
       </c>
       <c r="D75" s="2" t="str">
-        <f>C75</f>
+        <f t="shared" si="1"/>
         <v>jjfranch</v>
       </c>
       <c r="E75" s="23" t="str">
@@ -4321,7 +4349,7 @@
         <v>202</v>
       </c>
       <c r="D76" s="2" t="str">
-        <f>C76</f>
+        <f t="shared" si="1"/>
         <v>johnsmith</v>
       </c>
       <c r="E76" s="23" t="str">
@@ -4360,7 +4388,7 @@
         <v>205</v>
       </c>
       <c r="D77" s="2" t="str">
-        <f>C77</f>
+        <f t="shared" si="1"/>
         <v>neurolab</v>
       </c>
       <c r="E77" s="23" t="str">
@@ -4399,7 +4427,7 @@
         <v>207</v>
       </c>
       <c r="D78" s="2" t="str">
-        <f>C78</f>
+        <f t="shared" si="1"/>
         <v>gentech</v>
       </c>
       <c r="E78" s="23" t="str">
@@ -4438,7 +4466,7 @@
         <v>209</v>
       </c>
       <c r="D79" s="2" t="str">
-        <f>C79</f>
+        <f t="shared" si="1"/>
         <v>morg</v>
       </c>
       <c r="E79" s="23" t="str">
@@ -4477,7 +4505,7 @@
         <v>211</v>
       </c>
       <c r="D80" s="2" t="str">
-        <f>C80</f>
+        <f t="shared" si="1"/>
         <v>simbipet</v>
       </c>
       <c r="E80" s="23" t="str">
@@ -4554,7 +4582,7 @@
         <v>216</v>
       </c>
       <c r="D82" s="2" t="str">
-        <f>C82</f>
+        <f t="shared" ref="D82:D92" si="2">C82</f>
         <v>johnsmfund</v>
       </c>
       <c r="E82" s="23" t="str">
@@ -4593,7 +4621,7 @@
         <v>218</v>
       </c>
       <c r="D83" s="2" t="str">
-        <f>C83</f>
+        <f t="shared" si="2"/>
         <v>macfund</v>
       </c>
       <c r="E83" s="23" t="str">
@@ -4632,7 +4660,7 @@
         <v>220</v>
       </c>
       <c r="D84" s="2" t="str">
-        <f>C84</f>
+        <f t="shared" si="2"/>
         <v>kranfund</v>
       </c>
       <c r="E84" s="23" t="str">
@@ -4671,7 +4699,7 @@
         <v>222</v>
       </c>
       <c r="D85" s="2" t="str">
-        <f>C85</f>
+        <f t="shared" si="2"/>
         <v>gurfund</v>
       </c>
       <c r="E85" s="23" t="str">
@@ -4710,7 +4738,7 @@
         <v>224</v>
       </c>
       <c r="D86" s="2" t="str">
-        <f>C86</f>
+        <f t="shared" si="2"/>
         <v>jonsfund</v>
       </c>
       <c r="E86" s="23" t="str">
@@ -4749,7 +4777,7 @@
         <v>227</v>
       </c>
       <c r="D87" s="2" t="str">
-        <f>C87</f>
+        <f t="shared" si="2"/>
         <v>dinastfund</v>
       </c>
       <c r="E87" s="23" t="str">
@@ -4788,7 +4816,7 @@
         <v>229</v>
       </c>
       <c r="D88" s="2" t="str">
-        <f>C88</f>
+        <f t="shared" si="2"/>
         <v>investfund</v>
       </c>
       <c r="E88" s="23" t="str">
@@ -4827,7 +4855,7 @@
         <v>231</v>
       </c>
       <c r="D89" s="2" t="str">
-        <f>C89</f>
+        <f t="shared" si="2"/>
         <v>tradefund</v>
       </c>
       <c r="E89" s="23" t="str">
@@ -4866,7 +4894,7 @@
         <v>234</v>
       </c>
       <c r="D90" s="2" t="str">
-        <f>C90</f>
+        <f t="shared" si="2"/>
         <v>betcorn</v>
       </c>
       <c r="E90" s="23" t="str">
@@ -4905,7 +4933,7 @@
         <v>236</v>
       </c>
       <c r="D91" s="2" t="str">
-        <f>C91</f>
+        <f t="shared" si="2"/>
         <v>abyssclub</v>
       </c>
       <c r="E91" s="23" t="str">
@@ -4944,7 +4972,7 @@
         <v>238</v>
       </c>
       <c r="D92" s="2" t="str">
-        <f>C92</f>
+        <f t="shared" si="2"/>
         <v>highclub</v>
       </c>
       <c r="E92" s="23" t="str">
@@ -29496,10 +29524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -29682,6 +29710,29 @@
         <v>265</v>
       </c>
     </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29689,10 +29740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -29725,6 +29776,11 @@
         <v>248</v>
       </c>
     </row>
+    <row r="6" spans="1:2" ht="121" customHeight="1">
+      <c r="A6" s="33" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cash in game and cashout
</commit_message>
<xml_diff>
--- a/Company.xlsx
+++ b/Company.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="284">
   <si>
     <t>Старое название</t>
   </si>
@@ -819,9 +819,6 @@
     <t>Роль</t>
   </si>
   <si>
-    <t>Деньги</t>
-  </si>
-  <si>
     <t>Заведен</t>
   </si>
   <si>
@@ -29524,10 +29521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -29537,16 +29534,15 @@
     <col min="3" max="3" width="15.7265625" customWidth="1"/>
     <col min="4" max="4" width="19.453125" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1">
+    <row r="1" spans="1:6" s="30" customFormat="1">
       <c r="A1" s="31" t="s">
         <v>259</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>260</v>
@@ -29560,16 +29556,13 @@
       <c r="F1" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="G1" s="31" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="29" t="s">
         <v>253</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>250</v>
@@ -29580,37 +29573,31 @@
       <c r="E2" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="F2">
-        <v>1000000</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="29" t="s">
         <v>254</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>276</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>277</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="29" t="s">
         <v>256</v>
       </c>
@@ -29626,111 +29613,96 @@
       <c r="E4" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="F4">
-        <v>1000</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="29"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="29"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="29" t="s">
         <v>257</v>
       </c>
       <c r="B6" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>273</v>
-      </c>
       <c r="D6" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="F6">
-        <v>60000</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="29" t="s">
         <v>257</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>268</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="D7" t="s">
         <v>269</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="F7">
-        <v>300</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="13">
+      <c r="F7" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="29" t="s">
         <v>257</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="F8">
-        <v>1000</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F8" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" t="s">
         <v>279</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>280</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E10" t="s">
         <v>281</v>
       </c>
-      <c r="D10" t="s">
-        <v>283</v>
-      </c>
-      <c r="E10" t="s">
-        <v>282</v>
-      </c>
-      <c r="F10">
-        <v>1000</v>
-      </c>
-      <c r="G10" t="s">
-        <v>265</v>
+      <c r="F10" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -29742,7 +29714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -29778,7 +29750,7 @@
     </row>
     <row r="6" spans="1:2" ht="121" customHeight="1">
       <c r="A6" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>